<commit_message>
Added "ATDD.TestScriptor Format" column to ATTD sheets
</commit_message>
<xml_diff>
--- a/ATDD Scenarios/Clean sheet.xlsx
+++ b/ATDD Scenarios/Clean sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.178.68\fluxxus\Projects\Books\Packt\Contracts\Automated Testing in Microsoft Dynamics 365 Business Central\Source\Case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A470D69-49E4-4B9E-87A1-2100173A9F5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D63578-C745-43F0-B199-71C5EFC40A3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27585" windowHeight="12510" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="29610" yWindow="-1995" windowWidth="28110" windowHeight="18240" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>Feature</t>
   </si>
@@ -130,6 +131,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>ATDD.TestScriptor Format</t>
   </si>
 </sst>
 </file>
@@ -139,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +157,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -227,11 +237,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -272,16 +325,6 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -320,16 +363,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -344,46 +377,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:J6" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K6" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A1:K6" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:J18" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:J18" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:J18" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{EB12FABE-99EE-4C64-9371-664DA2BC018B}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{C4BF811B-A50B-4F15-ABFB-76F5EF61BAEC}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{CC6D9ED1-342A-442A-A781-19E1B48EC192}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="5">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,9 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -701,10 +739,11 @@
     <col min="7" max="7" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,10 +772,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -749,8 +791,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v xml:space="preserve">//[FEATURE] Feature </v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="17" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Feature' {</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -768,8 +814,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0001] Scenario</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="17" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0001 'Scenario' {</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -790,8 +840,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] A</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="17" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -812,8 +866,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] B</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="17" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'B'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -834,10 +892,14 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] C</v>
       </c>
+      <c r="J6" s="17" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'C' } }</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1338,7 +1400,7 @@
     <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>